<commit_message>
Figures probabilities for sample function.
Script figuring probailties of 2000 word chunks so that each
has equal chance of being sampled. Reduces frequency of Iliad
and Odyssey. The data are in parametersWithProbs,csv, the script is
probsForChunksOf2000.R.
</commit_message>
<xml_diff>
--- a/R_files/Rresults/Naive_Bayes_predictions/chunkSize2000/parameterForChunks.xlsx
+++ b/R_files/Rresults/Naive_Bayes_predictions/chunkSize2000/parameterForChunks.xlsx
@@ -4,17 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="18180" windowHeight="6830"/>
+    <workbookView xWindow="240" yWindow="90" windowWidth="18180" windowHeight="6825"/>
   </bookViews>
   <sheets>
     <sheet name="chunk_parameters" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="573">
   <si>
     <t>First</t>
   </si>
@@ -1712,13 +1712,34 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>Lysias</t>
+  </si>
+  <si>
+    <t>Odyssey</t>
+  </si>
+  <si>
+    <t>Plato</t>
+  </si>
+  <si>
+    <t>Plutarch</t>
+  </si>
+  <si>
+    <t>Polybius</t>
+  </si>
+  <si>
+    <t>Sophocles</t>
+  </si>
+  <si>
+    <t>Thucydides</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1853,6 +1874,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -2196,8 +2223,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2540,21 +2570,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G278"/>
+  <dimension ref="A1:J278"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="3.81640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="82.453125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="82.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="82.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="82.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>564</v>
       </c>
@@ -2574,7 +2604,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B2" t="s">
         <v>556</v>
       </c>
@@ -2593,8 +2626,15 @@
       <c r="G2">
         <v>2000</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <f>COUNT(C2:C26)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B3" t="s">
         <v>556</v>
       </c>
@@ -2614,7 +2654,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B4" t="s">
         <v>556</v>
       </c>
@@ -2634,7 +2677,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B5" t="s">
         <v>556</v>
       </c>
@@ -2654,7 +2700,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B6" t="s">
         <v>556</v>
       </c>
@@ -2674,7 +2723,10 @@
         <v>1527</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B7" t="s">
         <v>556</v>
       </c>
@@ -2694,7 +2746,10 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B8" t="s">
         <v>556</v>
       </c>
@@ -2714,7 +2769,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B9" t="s">
         <v>556</v>
       </c>
@@ -2734,7 +2792,10 @@
         <v>1502</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B10" t="s">
         <v>556</v>
       </c>
@@ -2754,7 +2815,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B11" t="s">
         <v>556</v>
       </c>
@@ -2774,7 +2838,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B12" t="s">
         <v>556</v>
       </c>
@@ -2794,7 +2861,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B13" t="s">
         <v>556</v>
       </c>
@@ -2814,7 +2884,10 @@
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B14" t="s">
         <v>556</v>
       </c>
@@ -2834,7 +2907,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B15" t="s">
         <v>556</v>
       </c>
@@ -2854,7 +2930,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B16" t="s">
         <v>556</v>
       </c>
@@ -2874,7 +2953,10 @@
         <v>1961</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B17" t="s">
         <v>556</v>
       </c>
@@ -2894,7 +2976,10 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B18" t="s">
         <v>556</v>
       </c>
@@ -2914,7 +2999,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B19" t="s">
         <v>556</v>
       </c>
@@ -2934,7 +3022,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B20" t="s">
         <v>556</v>
       </c>
@@ -2954,7 +3045,10 @@
         <v>824</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B21" t="s">
         <v>556</v>
       </c>
@@ -2974,7 +3068,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B22" t="s">
         <v>556</v>
       </c>
@@ -2994,7 +3091,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B23" t="s">
         <v>556</v>
       </c>
@@ -3014,7 +3114,10 @@
         <v>1974</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B24" t="s">
         <v>556</v>
       </c>
@@ -3034,7 +3137,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B25" t="s">
         <v>556</v>
       </c>
@@ -3054,7 +3160,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3.0769230000000001E-3</v>
+      </c>
       <c r="B26" t="s">
         <v>556</v>
       </c>
@@ -3074,7 +3183,10 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B27" t="s">
         <v>557</v>
       </c>
@@ -3093,8 +3205,15 @@
       <c r="G27">
         <v>2000</v>
       </c>
-    </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="J27" t="b">
+        <f>A27=COUNT(C27:C48)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B28" t="s">
         <v>557</v>
       </c>
@@ -3114,7 +3233,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B29" t="s">
         <v>557</v>
       </c>
@@ -3134,7 +3256,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B30" t="s">
         <v>557</v>
       </c>
@@ -3154,7 +3279,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B31" t="s">
         <v>557</v>
       </c>
@@ -3174,7 +3302,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B32" t="s">
         <v>557</v>
       </c>
@@ -3194,7 +3325,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B33" t="s">
         <v>557</v>
       </c>
@@ -3214,7 +3348,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="34" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B34" t="s">
         <v>557</v>
       </c>
@@ -3234,7 +3371,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B35" t="s">
         <v>557</v>
       </c>
@@ -3254,7 +3394,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B36" t="s">
         <v>557</v>
       </c>
@@ -3274,7 +3417,10 @@
         <v>1334</v>
       </c>
     </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B37" t="s">
         <v>557</v>
       </c>
@@ -3294,7 +3440,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B38" t="s">
         <v>557</v>
       </c>
@@ -3314,7 +3463,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B39" t="s">
         <v>557</v>
       </c>
@@ -3334,7 +3486,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B40" t="s">
         <v>557</v>
       </c>
@@ -3354,7 +3509,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B41" t="s">
         <v>557</v>
       </c>
@@ -3374,7 +3532,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B42" t="s">
         <v>557</v>
       </c>
@@ -3394,7 +3555,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B43" t="s">
         <v>557</v>
       </c>
@@ -3414,7 +3578,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B44" t="s">
         <v>557</v>
       </c>
@@ -3434,7 +3601,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B45" t="s">
         <v>557</v>
       </c>
@@ -3454,7 +3624,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B46" t="s">
         <v>557</v>
       </c>
@@ -3474,7 +3647,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B47" t="s">
         <v>557</v>
       </c>
@@ -3494,7 +3670,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>3.4965030000000002E-3</v>
+      </c>
       <c r="B48" t="s">
         <v>557</v>
       </c>
@@ -3514,7 +3693,10 @@
         <v>1781</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B49" t="s">
         <v>558</v>
       </c>
@@ -3534,7 +3716,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B50" t="s">
         <v>558</v>
       </c>
@@ -3554,7 +3739,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B51" t="s">
         <v>558</v>
       </c>
@@ -3574,7 +3762,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B52" t="s">
         <v>558</v>
       </c>
@@ -3594,7 +3785,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B53" t="s">
         <v>558</v>
       </c>
@@ -3614,7 +3808,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B54" t="s">
         <v>558</v>
       </c>
@@ -3634,7 +3831,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B55" t="s">
         <v>558</v>
       </c>
@@ -3654,7 +3854,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="56" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B56" t="s">
         <v>558</v>
       </c>
@@ -3674,7 +3877,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="57" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B57" t="s">
         <v>558</v>
       </c>
@@ -3694,7 +3900,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="58" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B58" t="s">
         <v>558</v>
       </c>
@@ -3714,7 +3923,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="59" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B59" t="s">
         <v>558</v>
       </c>
@@ -3734,7 +3946,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B60" t="s">
         <v>558</v>
       </c>
@@ -3754,7 +3969,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>5.9171600000000003E-3</v>
+      </c>
       <c r="B61" t="s">
         <v>558</v>
       </c>
@@ -3774,7 +3992,10 @@
         <v>223</v>
       </c>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B62" t="s">
         <v>559</v>
       </c>
@@ -3794,7 +4015,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B63" t="s">
         <v>559</v>
       </c>
@@ -3814,7 +4038,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="64" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B64" t="s">
         <v>559</v>
       </c>
@@ -3834,7 +4061,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B65" t="s">
         <v>559</v>
       </c>
@@ -3854,7 +4084,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B66" t="s">
         <v>559</v>
       </c>
@@ -3874,7 +4107,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B67" t="s">
         <v>559</v>
       </c>
@@ -3894,7 +4130,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B68" t="s">
         <v>559</v>
       </c>
@@ -3914,7 +4153,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="69" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B69" t="s">
         <v>559</v>
       </c>
@@ -3934,7 +4176,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="70" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B70" t="s">
         <v>559</v>
       </c>
@@ -3954,7 +4199,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="71" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B71" t="s">
         <v>559</v>
       </c>
@@ -3974,7 +4222,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="72" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B72" t="s">
         <v>559</v>
       </c>
@@ -3994,7 +4245,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="73" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B73" t="s">
         <v>559</v>
       </c>
@@ -4014,7 +4268,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="74" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B74" t="s">
         <v>559</v>
       </c>
@@ -4034,7 +4291,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="75" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B75" t="s">
         <v>559</v>
       </c>
@@ -4054,7 +4314,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B76" t="s">
         <v>559</v>
       </c>
@@ -4074,7 +4337,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="77" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="1">
+        <v>4.8076919999999997E-3</v>
+      </c>
       <c r="B77" t="s">
         <v>559</v>
       </c>
@@ -4094,7 +4360,10 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="78" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B78" t="s">
         <v>560</v>
       </c>
@@ -4114,7 +4383,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="79" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B79" t="s">
         <v>560</v>
       </c>
@@ -4134,7 +4406,10 @@
         <v>1705</v>
       </c>
     </row>
-    <row r="80" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B80" t="s">
         <v>560</v>
       </c>
@@ -4154,7 +4429,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="81" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B81" t="s">
         <v>560</v>
       </c>
@@ -4174,7 +4452,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="82" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B82" t="s">
         <v>560</v>
       </c>
@@ -4194,7 +4475,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="83" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B83" t="s">
         <v>560</v>
       </c>
@@ -4214,7 +4498,10 @@
         <v>1761</v>
       </c>
     </row>
-    <row r="84" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B84" t="s">
         <v>560</v>
       </c>
@@ -4234,7 +4521,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="85" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B85" t="s">
         <v>560</v>
       </c>
@@ -4254,7 +4544,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="86" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B86" t="s">
         <v>560</v>
       </c>
@@ -4274,7 +4567,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="87" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>7.6923080000000001E-3</v>
+      </c>
       <c r="B87" t="s">
         <v>560</v>
       </c>
@@ -4293,8 +4589,15 @@
       <c r="G87">
         <v>654</v>
       </c>
-    </row>
-    <row r="88" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="I87">
+        <f>COUNT(C88:C152,C187:C195)</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B88" t="s">
         <v>561</v>
       </c>
@@ -4314,7 +4617,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="89" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B89" t="s">
         <v>561</v>
       </c>
@@ -4334,7 +4640,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="90" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B90" t="s">
         <v>561</v>
       </c>
@@ -4354,7 +4663,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="91" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B91" t="s">
         <v>561</v>
       </c>
@@ -4374,7 +4686,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="92" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B92" t="s">
         <v>561</v>
       </c>
@@ -4394,7 +4709,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="93" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B93" t="s">
         <v>561</v>
       </c>
@@ -4414,7 +4732,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="94" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B94" t="s">
         <v>561</v>
       </c>
@@ -4434,7 +4755,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="95" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B95" t="s">
         <v>561</v>
       </c>
@@ -4454,7 +4778,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="96" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B96" t="s">
         <v>561</v>
       </c>
@@ -4474,7 +4801,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="97" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B97" t="s">
         <v>561</v>
       </c>
@@ -4494,7 +4824,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="98" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B98" t="s">
         <v>561</v>
       </c>
@@ -4514,7 +4847,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="99" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B99" t="s">
         <v>561</v>
       </c>
@@ -4534,7 +4870,10 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="100" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B100" t="s">
         <v>561</v>
       </c>
@@ -4554,7 +4893,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="101" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B101" t="s">
         <v>561</v>
       </c>
@@ -4574,7 +4916,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="102" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B102" t="s">
         <v>561</v>
       </c>
@@ -4594,7 +4939,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="103" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B103" t="s">
         <v>561</v>
       </c>
@@ -4614,7 +4962,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="104" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B104" t="s">
         <v>561</v>
       </c>
@@ -4634,7 +4985,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="105" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B105" t="s">
         <v>561</v>
       </c>
@@ -4654,7 +5008,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="106" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B106" t="s">
         <v>561</v>
       </c>
@@ -4674,7 +5031,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="107" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B107" t="s">
         <v>561</v>
       </c>
@@ -4694,7 +5054,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="108" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B108" t="s">
         <v>561</v>
       </c>
@@ -4714,7 +5077,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="109" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B109" t="s">
         <v>561</v>
       </c>
@@ -4734,7 +5100,10 @@
         <v>1520</v>
       </c>
     </row>
-    <row r="110" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B110" t="s">
         <v>561</v>
       </c>
@@ -4754,7 +5123,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="111" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B111" t="s">
         <v>561</v>
       </c>
@@ -4774,7 +5146,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="112" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B112" t="s">
         <v>561</v>
       </c>
@@ -4794,7 +5169,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="113" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B113" t="s">
         <v>561</v>
       </c>
@@ -4814,7 +5192,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="114" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B114" t="s">
         <v>561</v>
       </c>
@@ -4834,7 +5215,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="115" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B115" t="s">
         <v>561</v>
       </c>
@@ -4854,7 +5238,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="116" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B116" t="s">
         <v>561</v>
       </c>
@@ -4874,7 +5261,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="117" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B117" t="s">
         <v>561</v>
       </c>
@@ -4894,7 +5284,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="118" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B118" t="s">
         <v>561</v>
       </c>
@@ -4914,7 +5307,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="119" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B119" t="s">
         <v>561</v>
       </c>
@@ -4934,7 +5330,10 @@
         <v>183</v>
       </c>
     </row>
-    <row r="120" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B120" t="s">
         <v>561</v>
       </c>
@@ -4954,7 +5353,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="121" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B121" t="s">
         <v>561</v>
       </c>
@@ -4974,7 +5376,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="122" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B122" t="s">
         <v>561</v>
       </c>
@@ -4994,7 +5399,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="123" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B123" t="s">
         <v>561</v>
       </c>
@@ -5014,7 +5422,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="124" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B124" t="s">
         <v>561</v>
       </c>
@@ -5034,7 +5445,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="125" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B125" t="s">
         <v>561</v>
       </c>
@@ -5054,7 +5468,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="126" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B126" t="s">
         <v>561</v>
       </c>
@@ -5074,7 +5491,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="127" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B127" t="s">
         <v>561</v>
       </c>
@@ -5094,7 +5514,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="128" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B128" t="s">
         <v>561</v>
       </c>
@@ -5114,7 +5537,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="129" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B129" t="s">
         <v>561</v>
       </c>
@@ -5134,7 +5560,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="130" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B130" t="s">
         <v>561</v>
       </c>
@@ -5154,7 +5583,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="131" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B131" t="s">
         <v>561</v>
       </c>
@@ -5174,7 +5606,10 @@
         <v>738</v>
       </c>
     </row>
-    <row r="132" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B132" t="s">
         <v>561</v>
       </c>
@@ -5194,7 +5629,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="133" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B133" t="s">
         <v>561</v>
       </c>
@@ -5214,7 +5652,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="134" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B134" t="s">
         <v>561</v>
       </c>
@@ -5234,7 +5675,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="135" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B135" t="s">
         <v>561</v>
       </c>
@@ -5254,7 +5698,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="136" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B136" t="s">
         <v>561</v>
       </c>
@@ -5274,7 +5721,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="137" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B137" t="s">
         <v>561</v>
       </c>
@@ -5294,7 +5744,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="138" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B138" t="s">
         <v>561</v>
       </c>
@@ -5314,7 +5767,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="139" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B139" t="s">
         <v>561</v>
       </c>
@@ -5334,7 +5790,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="140" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B140" t="s">
         <v>561</v>
       </c>
@@ -5354,7 +5813,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="141" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A141" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B141" t="s">
         <v>561</v>
       </c>
@@ -5374,7 +5836,10 @@
         <v>1473</v>
       </c>
     </row>
-    <row r="142" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A142" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B142" t="s">
         <v>561</v>
       </c>
@@ -5394,7 +5859,10 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="143" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A143" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B143" t="s">
         <v>561</v>
       </c>
@@ -5414,7 +5882,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="144" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A144" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B144" t="s">
         <v>561</v>
       </c>
@@ -5434,7 +5905,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="145" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A145" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B145" t="s">
         <v>561</v>
       </c>
@@ -5454,7 +5928,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="146" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A146" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B146" t="s">
         <v>561</v>
       </c>
@@ -5474,7 +5951,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="147" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A147" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B147" t="s">
         <v>561</v>
       </c>
@@ -5494,7 +5974,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="148" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A148" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B148" t="s">
         <v>561</v>
       </c>
@@ -5514,7 +5997,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="149" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A149" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B149" t="s">
         <v>561</v>
       </c>
@@ -5534,7 +6020,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="150" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A150" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B150" t="s">
         <v>561</v>
       </c>
@@ -5554,7 +6043,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="151" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A151" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B151" t="s">
         <v>561</v>
       </c>
@@ -5574,7 +6066,10 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="152" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A152" s="1">
+        <v>1.039501E-3</v>
+      </c>
       <c r="B152" t="s">
         <v>561</v>
       </c>
@@ -5594,7 +6089,16 @@
         <v>662</v>
       </c>
     </row>
-    <row r="153" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A153" s="1">
+        <v>1.282051E-2</v>
+      </c>
+      <c r="B153" t="s">
+        <v>566</v>
+      </c>
+      <c r="C153">
+        <v>1</v>
+      </c>
       <c r="D153">
         <v>152</v>
       </c>
@@ -5608,7 +6112,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="154" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A154" s="1">
+        <v>1.282051E-2</v>
+      </c>
+      <c r="B154" t="s">
+        <v>566</v>
+      </c>
+      <c r="C154">
+        <v>2</v>
+      </c>
       <c r="D154">
         <v>153</v>
       </c>
@@ -5622,7 +6135,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="155" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A155" s="1">
+        <v>1.282051E-2</v>
+      </c>
+      <c r="B155" t="s">
+        <v>566</v>
+      </c>
+      <c r="C155">
+        <v>3</v>
+      </c>
       <c r="D155">
         <v>154</v>
       </c>
@@ -5636,7 +6158,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="156" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A156" s="1">
+        <v>1.282051E-2</v>
+      </c>
+      <c r="B156" t="s">
+        <v>566</v>
+      </c>
+      <c r="C156">
+        <v>4</v>
+      </c>
       <c r="D156">
         <v>155</v>
       </c>
@@ -5650,7 +6181,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="157" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A157" s="1">
+        <v>1.282051E-2</v>
+      </c>
+      <c r="B157" t="s">
+        <v>566</v>
+      </c>
+      <c r="C157">
+        <v>5</v>
+      </c>
       <c r="D157">
         <v>156</v>
       </c>
@@ -5664,7 +6204,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="158" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A158" s="1">
+        <v>1.282051E-2</v>
+      </c>
+      <c r="B158" t="s">
+        <v>566</v>
+      </c>
+      <c r="C158">
+        <v>6</v>
+      </c>
       <c r="D158">
         <v>157</v>
       </c>
@@ -5678,7 +6227,16 @@
         <v>1868</v>
       </c>
     </row>
-    <row r="159" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A159" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B159" t="s">
+        <v>567</v>
+      </c>
+      <c r="C159">
+        <v>1</v>
+      </c>
       <c r="D159">
         <v>158</v>
       </c>
@@ -5692,7 +6250,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="160" spans="2:7" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A160" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B160" t="s">
+        <v>567</v>
+      </c>
+      <c r="C160">
+        <v>2</v>
+      </c>
       <c r="D160">
         <v>159</v>
       </c>
@@ -5705,8 +6272,21 @@
       <c r="G160">
         <v>2000</v>
       </c>
-    </row>
-    <row r="161" spans="4:7" x14ac:dyDescent="0.35">
+      <c r="I160">
+        <f>COUNT(C159:C186,C196:C211)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B161" t="s">
+        <v>567</v>
+      </c>
+      <c r="C161">
+        <v>3</v>
+      </c>
       <c r="D161">
         <v>160</v>
       </c>
@@ -5720,7 +6300,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="162" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A162" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>567</v>
+      </c>
+      <c r="C162">
+        <v>4</v>
+      </c>
       <c r="D162">
         <v>161</v>
       </c>
@@ -5734,7 +6323,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="163" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A163" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B163" t="s">
+        <v>567</v>
+      </c>
+      <c r="C163">
+        <v>5</v>
+      </c>
       <c r="D163">
         <v>162</v>
       </c>
@@ -5748,7 +6346,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="164" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A164" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B164" t="s">
+        <v>567</v>
+      </c>
+      <c r="C164">
+        <v>6</v>
+      </c>
       <c r="D164">
         <v>163</v>
       </c>
@@ -5762,7 +6369,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="165" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A165" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B165" t="s">
+        <v>567</v>
+      </c>
+      <c r="C165">
+        <v>7</v>
+      </c>
       <c r="D165">
         <v>164</v>
       </c>
@@ -5776,7 +6392,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="166" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A166" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B166" t="s">
+        <v>567</v>
+      </c>
+      <c r="C166">
+        <v>8</v>
+      </c>
       <c r="D166">
         <v>165</v>
       </c>
@@ -5790,7 +6415,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="167" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A167" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B167" t="s">
+        <v>567</v>
+      </c>
+      <c r="C167">
+        <v>9</v>
+      </c>
       <c r="D167">
         <v>166</v>
       </c>
@@ -5804,7 +6438,16 @@
         <v>1955</v>
       </c>
     </row>
-    <row r="168" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A168" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B168" t="s">
+        <v>567</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
       <c r="D168">
         <v>167</v>
       </c>
@@ -5818,7 +6461,16 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="169" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A169" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B169" t="s">
+        <v>567</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
       <c r="D169">
         <v>168</v>
       </c>
@@ -5832,7 +6484,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="170" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A170" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B170" t="s">
+        <v>567</v>
+      </c>
+      <c r="C170">
+        <v>3</v>
+      </c>
       <c r="D170">
         <v>169</v>
       </c>
@@ -5846,7 +6507,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="171" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A171" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B171" t="s">
+        <v>567</v>
+      </c>
+      <c r="C171">
+        <v>4</v>
+      </c>
       <c r="D171">
         <v>170</v>
       </c>
@@ -5860,7 +6530,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="172" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A172" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B172" t="s">
+        <v>567</v>
+      </c>
+      <c r="C172">
+        <v>5</v>
+      </c>
       <c r="D172">
         <v>171</v>
       </c>
@@ -5874,7 +6553,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="173" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A173" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B173" t="s">
+        <v>567</v>
+      </c>
+      <c r="C173">
+        <v>6</v>
+      </c>
       <c r="D173">
         <v>172</v>
       </c>
@@ -5888,7 +6576,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="174" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A174" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B174" t="s">
+        <v>567</v>
+      </c>
+      <c r="C174">
+        <v>7</v>
+      </c>
       <c r="D174">
         <v>173</v>
       </c>
@@ -5902,7 +6599,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="175" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A175" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B175" t="s">
+        <v>567</v>
+      </c>
+      <c r="C175">
+        <v>8</v>
+      </c>
       <c r="D175">
         <v>174</v>
       </c>
@@ -5916,7 +6622,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="176" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A176" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B176" t="s">
+        <v>567</v>
+      </c>
+      <c r="C176">
+        <v>9</v>
+      </c>
       <c r="D176">
         <v>175</v>
       </c>
@@ -5930,7 +6645,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="177" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A177" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B177" t="s">
+        <v>567</v>
+      </c>
+      <c r="C177">
+        <v>10</v>
+      </c>
       <c r="D177">
         <v>176</v>
       </c>
@@ -5944,7 +6668,16 @@
         <v>66</v>
       </c>
     </row>
-    <row r="178" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A178" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B178" t="s">
+        <v>567</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
       <c r="D178">
         <v>177</v>
       </c>
@@ -5958,7 +6691,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="179" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A179" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B179" t="s">
+        <v>567</v>
+      </c>
+      <c r="C179">
+        <v>2</v>
+      </c>
       <c r="D179">
         <v>178</v>
       </c>
@@ -5972,7 +6714,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="180" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A180" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B180" t="s">
+        <v>567</v>
+      </c>
+      <c r="C180">
+        <v>3</v>
+      </c>
       <c r="D180">
         <v>179</v>
       </c>
@@ -5986,7 +6737,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="181" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A181" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B181" t="s">
+        <v>567</v>
+      </c>
+      <c r="C181">
+        <v>4</v>
+      </c>
       <c r="D181">
         <v>180</v>
       </c>
@@ -6000,7 +6760,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="182" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A182" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B182" t="s">
+        <v>567</v>
+      </c>
+      <c r="C182">
+        <v>5</v>
+      </c>
       <c r="D182">
         <v>181</v>
       </c>
@@ -6014,7 +6783,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="183" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A183" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B183" t="s">
+        <v>567</v>
+      </c>
+      <c r="C183">
+        <v>6</v>
+      </c>
       <c r="D183">
         <v>182</v>
       </c>
@@ -6028,7 +6806,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="184" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A184" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>567</v>
+      </c>
+      <c r="C184">
+        <v>7</v>
+      </c>
       <c r="D184">
         <v>183</v>
       </c>
@@ -6042,7 +6829,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="185" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A185" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B185" t="s">
+        <v>567</v>
+      </c>
+      <c r="C185">
+        <v>8</v>
+      </c>
       <c r="D185">
         <v>184</v>
       </c>
@@ -6056,7 +6852,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="186" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A186" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B186" t="s">
+        <v>567</v>
+      </c>
+      <c r="C186">
+        <v>9</v>
+      </c>
       <c r="D186">
         <v>185</v>
       </c>
@@ -6070,7 +6875,16 @@
         <v>406</v>
       </c>
     </row>
-    <row r="187" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A187" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B187" t="s">
+        <v>561</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
       <c r="D187">
         <v>186</v>
       </c>
@@ -6084,7 +6898,16 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="188" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A188" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B188" t="s">
+        <v>561</v>
+      </c>
+      <c r="C188">
+        <v>2</v>
+      </c>
       <c r="D188">
         <v>187</v>
       </c>
@@ -6098,7 +6921,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="189" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A189" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B189" t="s">
+        <v>561</v>
+      </c>
+      <c r="C189">
+        <v>3</v>
+      </c>
       <c r="D189">
         <v>188</v>
       </c>
@@ -6112,7 +6944,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="190" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A190" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B190" t="s">
+        <v>561</v>
+      </c>
+      <c r="C190">
+        <v>4</v>
+      </c>
       <c r="D190">
         <v>189</v>
       </c>
@@ -6126,7 +6967,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="191" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A191" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B191" t="s">
+        <v>561</v>
+      </c>
+      <c r="C191">
+        <v>5</v>
+      </c>
       <c r="D191">
         <v>190</v>
       </c>
@@ -6140,7 +6990,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="192" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A192" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B192" t="s">
+        <v>561</v>
+      </c>
+      <c r="C192">
+        <v>6</v>
+      </c>
       <c r="D192">
         <v>191</v>
       </c>
@@ -6154,7 +7013,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="193" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A193" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B193" t="s">
+        <v>561</v>
+      </c>
+      <c r="C193">
+        <v>7</v>
+      </c>
       <c r="D193">
         <v>192</v>
       </c>
@@ -6168,7 +7036,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="194" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A194" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B194" t="s">
+        <v>561</v>
+      </c>
+      <c r="C194">
+        <v>8</v>
+      </c>
       <c r="D194">
         <v>193</v>
       </c>
@@ -6182,7 +7059,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="195" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A195" s="1">
+        <v>1.039501E-3</v>
+      </c>
+      <c r="B195" t="s">
+        <v>561</v>
+      </c>
+      <c r="C195">
+        <v>9</v>
+      </c>
       <c r="D195">
         <v>194</v>
       </c>
@@ -6196,7 +7082,16 @@
         <v>633</v>
       </c>
     </row>
-    <row r="196" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A196" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B196" t="s">
+        <v>567</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
       <c r="D196">
         <v>195</v>
       </c>
@@ -6210,7 +7105,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="197" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A197" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B197" t="s">
+        <v>567</v>
+      </c>
+      <c r="C197">
+        <v>2</v>
+      </c>
       <c r="D197">
         <v>196</v>
       </c>
@@ -6224,7 +7128,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="198" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A198" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B198" t="s">
+        <v>567</v>
+      </c>
+      <c r="C198">
+        <v>3</v>
+      </c>
       <c r="D198">
         <v>197</v>
       </c>
@@ -6238,7 +7151,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="199" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A199" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B199" t="s">
+        <v>567</v>
+      </c>
+      <c r="C199">
+        <v>4</v>
+      </c>
       <c r="D199">
         <v>198</v>
       </c>
@@ -6252,7 +7174,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="200" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A200" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B200" t="s">
+        <v>567</v>
+      </c>
+      <c r="C200">
+        <v>5</v>
+      </c>
       <c r="D200">
         <v>199</v>
       </c>
@@ -6266,7 +7197,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="201" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A201" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B201" t="s">
+        <v>567</v>
+      </c>
+      <c r="C201">
+        <v>6</v>
+      </c>
       <c r="D201">
         <v>200</v>
       </c>
@@ -6280,7 +7220,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="202" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A202" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B202" t="s">
+        <v>567</v>
+      </c>
+      <c r="C202">
+        <v>7</v>
+      </c>
       <c r="D202">
         <v>201</v>
       </c>
@@ -6294,7 +7243,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="203" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A203" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B203" t="s">
+        <v>567</v>
+      </c>
+      <c r="C203">
+        <v>8</v>
+      </c>
       <c r="D203">
         <v>202</v>
       </c>
@@ -6308,7 +7266,16 @@
         <v>853</v>
       </c>
     </row>
-    <row r="204" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A204" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B204" t="s">
+        <v>567</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
       <c r="D204">
         <v>203</v>
       </c>
@@ -6322,7 +7289,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="205" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A205" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B205" t="s">
+        <v>567</v>
+      </c>
+      <c r="C205">
+        <v>2</v>
+      </c>
       <c r="D205">
         <v>204</v>
       </c>
@@ -6336,7 +7312,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="206" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A206" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B206" t="s">
+        <v>567</v>
+      </c>
+      <c r="C206">
+        <v>3</v>
+      </c>
       <c r="D206">
         <v>205</v>
       </c>
@@ -6350,7 +7335,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="207" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A207" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B207" t="s">
+        <v>567</v>
+      </c>
+      <c r="C207">
+        <v>4</v>
+      </c>
       <c r="D207">
         <v>206</v>
       </c>
@@ -6364,7 +7358,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="208" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A208" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B208" t="s">
+        <v>567</v>
+      </c>
+      <c r="C208">
+        <v>5</v>
+      </c>
       <c r="D208">
         <v>207</v>
       </c>
@@ -6378,7 +7381,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="209" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A209" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B209" t="s">
+        <v>567</v>
+      </c>
+      <c r="C209">
+        <v>6</v>
+      </c>
       <c r="D209">
         <v>208</v>
       </c>
@@ -6392,7 +7404,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="210" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A210" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B210" t="s">
+        <v>567</v>
+      </c>
+      <c r="C210">
+        <v>7</v>
+      </c>
       <c r="D210">
         <v>209</v>
       </c>
@@ -6406,7 +7427,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="211" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A211" s="1">
+        <v>1.7482520000000001E-3</v>
+      </c>
+      <c r="B211" t="s">
+        <v>567</v>
+      </c>
+      <c r="C211">
+        <v>8</v>
+      </c>
       <c r="D211">
         <v>210</v>
       </c>
@@ -6420,7 +7450,16 @@
         <v>318</v>
       </c>
     </row>
-    <row r="212" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A212" s="1">
+        <v>2.5641029999999999E-2</v>
+      </c>
+      <c r="B212" t="s">
+        <v>568</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
       <c r="D212">
         <v>211</v>
       </c>
@@ -6434,7 +7473,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="213" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A213" s="1">
+        <v>2.5641029999999999E-2</v>
+      </c>
+      <c r="B213" t="s">
+        <v>568</v>
+      </c>
+      <c r="C213">
+        <v>2</v>
+      </c>
       <c r="D213">
         <v>212</v>
       </c>
@@ -6448,7 +7496,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="214" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A214" s="1">
+        <v>2.5641029999999999E-2</v>
+      </c>
+      <c r="B214" t="s">
+        <v>568</v>
+      </c>
+      <c r="C214">
+        <v>3</v>
+      </c>
       <c r="D214">
         <v>213</v>
       </c>
@@ -6462,7 +7519,16 @@
         <v>1882</v>
       </c>
     </row>
-    <row r="215" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A215" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B215" t="s">
+        <v>569</v>
+      </c>
+      <c r="C215">
+        <v>1</v>
+      </c>
       <c r="D215">
         <v>214</v>
       </c>
@@ -6476,7 +7542,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="216" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A216" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B216" t="s">
+        <v>569</v>
+      </c>
+      <c r="C216">
+        <v>2</v>
+      </c>
       <c r="D216">
         <v>215</v>
       </c>
@@ -6490,7 +7565,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="217" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A217" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B217" t="s">
+        <v>569</v>
+      </c>
+      <c r="C217">
+        <v>3</v>
+      </c>
       <c r="D217">
         <v>216</v>
       </c>
@@ -6504,7 +7588,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="218" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A218" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B218" t="s">
+        <v>569</v>
+      </c>
+      <c r="C218">
+        <v>4</v>
+      </c>
       <c r="D218">
         <v>217</v>
       </c>
@@ -6518,7 +7611,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="219" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A219" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B219" t="s">
+        <v>569</v>
+      </c>
+      <c r="C219">
+        <v>5</v>
+      </c>
       <c r="D219">
         <v>218</v>
       </c>
@@ -6532,7 +7634,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="220" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A220" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B220" t="s">
+        <v>569</v>
+      </c>
+      <c r="C220">
+        <v>6</v>
+      </c>
       <c r="D220">
         <v>219</v>
       </c>
@@ -6546,7 +7657,16 @@
         <v>640</v>
       </c>
     </row>
-    <row r="221" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A221" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B221" t="s">
+        <v>569</v>
+      </c>
+      <c r="C221">
+        <v>1</v>
+      </c>
       <c r="D221">
         <v>220</v>
       </c>
@@ -6560,7 +7680,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="222" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A222" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B222" t="s">
+        <v>569</v>
+      </c>
+      <c r="C222">
+        <v>2</v>
+      </c>
       <c r="D222">
         <v>221</v>
       </c>
@@ -6574,7 +7703,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="223" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A223" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B223" t="s">
+        <v>569</v>
+      </c>
+      <c r="C223">
+        <v>3</v>
+      </c>
       <c r="D223">
         <v>222</v>
       </c>
@@ -6588,7 +7726,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="224" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A224" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B224" t="s">
+        <v>569</v>
+      </c>
+      <c r="C224">
+        <v>4</v>
+      </c>
       <c r="D224">
         <v>223</v>
       </c>
@@ -6602,7 +7749,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="225" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A225" s="1">
+        <v>6.9930069999999999E-3</v>
+      </c>
+      <c r="B225" t="s">
+        <v>569</v>
+      </c>
+      <c r="C225">
+        <v>5</v>
+      </c>
       <c r="D225">
         <v>224</v>
       </c>
@@ -6616,7 +7772,16 @@
         <v>1996</v>
       </c>
     </row>
-    <row r="226" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A226" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B226" t="s">
+        <v>570</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
       <c r="D226">
         <v>225</v>
       </c>
@@ -6630,7 +7795,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="227" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A227" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B227" t="s">
+        <v>570</v>
+      </c>
+      <c r="C227">
+        <v>2</v>
+      </c>
       <c r="D227">
         <v>226</v>
       </c>
@@ -6644,7 +7818,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="228" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A228" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B228" t="s">
+        <v>570</v>
+      </c>
+      <c r="C228">
+        <v>3</v>
+      </c>
       <c r="D228">
         <v>227</v>
       </c>
@@ -6658,7 +7841,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="229" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A229" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B229" t="s">
+        <v>570</v>
+      </c>
+      <c r="C229">
+        <v>4</v>
+      </c>
       <c r="D229">
         <v>228</v>
       </c>
@@ -6672,7 +7864,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="230" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A230" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B230" t="s">
+        <v>570</v>
+      </c>
+      <c r="C230">
+        <v>5</v>
+      </c>
       <c r="D230">
         <v>229</v>
       </c>
@@ -6686,7 +7887,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="231" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A231" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B231" t="s">
+        <v>570</v>
+      </c>
+      <c r="C231">
+        <v>6</v>
+      </c>
       <c r="D231">
         <v>230</v>
       </c>
@@ -6700,7 +7910,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="232" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A232" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B232" t="s">
+        <v>570</v>
+      </c>
+      <c r="C232">
+        <v>7</v>
+      </c>
       <c r="D232">
         <v>231</v>
       </c>
@@ -6714,7 +7933,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="233" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A233" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B233" t="s">
+        <v>570</v>
+      </c>
+      <c r="C233">
+        <v>8</v>
+      </c>
       <c r="D233">
         <v>232</v>
       </c>
@@ -6728,7 +7956,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="234" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A234" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B234" t="s">
+        <v>570</v>
+      </c>
+      <c r="C234">
+        <v>9</v>
+      </c>
       <c r="D234">
         <v>233</v>
       </c>
@@ -6742,7 +7979,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="235" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A235" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B235" t="s">
+        <v>570</v>
+      </c>
+      <c r="C235">
+        <v>10</v>
+      </c>
       <c r="D235">
         <v>234</v>
       </c>
@@ -6756,7 +8002,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="236" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A236" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B236" t="s">
+        <v>570</v>
+      </c>
+      <c r="C236">
+        <v>11</v>
+      </c>
       <c r="D236">
         <v>235</v>
       </c>
@@ -6770,7 +8025,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="237" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A237" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B237" t="s">
+        <v>570</v>
+      </c>
+      <c r="C237">
+        <v>12</v>
+      </c>
       <c r="D237">
         <v>236</v>
       </c>
@@ -6784,7 +8048,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="238" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A238" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B238" t="s">
+        <v>570</v>
+      </c>
+      <c r="C238">
+        <v>13</v>
+      </c>
       <c r="D238">
         <v>237</v>
       </c>
@@ -6798,7 +8071,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="239" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A239" s="1">
+        <v>5.4945050000000002E-3</v>
+      </c>
+      <c r="B239" t="s">
+        <v>570</v>
+      </c>
+      <c r="C239">
+        <v>14</v>
+      </c>
       <c r="D239">
         <v>238</v>
       </c>
@@ -6812,7 +8094,16 @@
         <v>894</v>
       </c>
     </row>
-    <row r="240" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A240" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B240" t="s">
+        <v>571</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
       <c r="D240">
         <v>239</v>
       </c>
@@ -6826,7 +8117,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="241" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A241" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B241" t="s">
+        <v>571</v>
+      </c>
+      <c r="C241">
+        <v>2</v>
+      </c>
       <c r="D241">
         <v>240</v>
       </c>
@@ -6840,7 +8140,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="242" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B242" t="s">
+        <v>571</v>
+      </c>
+      <c r="C242">
+        <v>3</v>
+      </c>
       <c r="D242">
         <v>241</v>
       </c>
@@ -6854,7 +8163,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="243" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B243" t="s">
+        <v>571</v>
+      </c>
+      <c r="C243">
+        <v>4</v>
+      </c>
       <c r="D243">
         <v>242</v>
       </c>
@@ -6868,7 +8186,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="244" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B244" t="s">
+        <v>571</v>
+      </c>
+      <c r="C244">
+        <v>5</v>
+      </c>
       <c r="D244">
         <v>243</v>
       </c>
@@ -6882,7 +8209,16 @@
         <v>1110</v>
       </c>
     </row>
-    <row r="245" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B245" t="s">
+        <v>571</v>
+      </c>
+      <c r="C245">
+        <v>1</v>
+      </c>
       <c r="D245">
         <v>244</v>
       </c>
@@ -6896,7 +8232,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="246" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B246" t="s">
+        <v>571</v>
+      </c>
+      <c r="C246">
+        <v>2</v>
+      </c>
       <c r="D246">
         <v>245</v>
       </c>
@@ -6910,7 +8255,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="247" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B247" t="s">
+        <v>571</v>
+      </c>
+      <c r="C247">
+        <v>3</v>
+      </c>
       <c r="D247">
         <v>246</v>
       </c>
@@ -6924,7 +8278,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="248" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B248" t="s">
+        <v>571</v>
+      </c>
+      <c r="C248">
+        <v>4</v>
+      </c>
       <c r="D248">
         <v>247</v>
       </c>
@@ -6938,7 +8301,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="249" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B249" t="s">
+        <v>571</v>
+      </c>
+      <c r="C249">
+        <v>5</v>
+      </c>
       <c r="D249">
         <v>248</v>
       </c>
@@ -6952,7 +8324,16 @@
         <v>443</v>
       </c>
     </row>
-    <row r="250" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B250" t="s">
+        <v>571</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
       <c r="D250">
         <v>249</v>
       </c>
@@ -6966,7 +8347,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="251" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B251" t="s">
+        <v>571</v>
+      </c>
+      <c r="C251">
+        <v>2</v>
+      </c>
       <c r="D251">
         <v>250</v>
       </c>
@@ -6980,7 +8370,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="252" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B252" t="s">
+        <v>571</v>
+      </c>
+      <c r="C252">
+        <v>3</v>
+      </c>
       <c r="D252">
         <v>251</v>
       </c>
@@ -6994,7 +8393,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="253" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B253" t="s">
+        <v>571</v>
+      </c>
+      <c r="C253">
+        <v>4</v>
+      </c>
       <c r="D253">
         <v>252</v>
       </c>
@@ -7008,7 +8416,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="254" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B254" t="s">
+        <v>571</v>
+      </c>
+      <c r="C254">
+        <v>5</v>
+      </c>
       <c r="D254">
         <v>253</v>
       </c>
@@ -7022,7 +8439,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="255" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B255" t="s">
+        <v>571</v>
+      </c>
+      <c r="C255">
+        <v>6</v>
+      </c>
       <c r="D255">
         <v>254</v>
       </c>
@@ -7036,7 +8462,16 @@
         <v>121</v>
       </c>
     </row>
-    <row r="256" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A256" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B256" t="s">
+        <v>571</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
       <c r="D256">
         <v>255</v>
       </c>
@@ -7050,7 +8485,16 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="257" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A257" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B257" t="s">
+        <v>571</v>
+      </c>
+      <c r="C257">
+        <v>2</v>
+      </c>
       <c r="D257">
         <v>256</v>
       </c>
@@ -7064,7 +8508,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="258" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A258" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B258" t="s">
+        <v>571</v>
+      </c>
+      <c r="C258">
+        <v>3</v>
+      </c>
       <c r="D258">
         <v>257</v>
       </c>
@@ -7078,7 +8531,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="259" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A259" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B259" t="s">
+        <v>571</v>
+      </c>
+      <c r="C259">
+        <v>4</v>
+      </c>
       <c r="D259">
         <v>258</v>
       </c>
@@ -7092,7 +8554,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="260" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A260" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B260" t="s">
+        <v>571</v>
+      </c>
+      <c r="C260">
+        <v>5</v>
+      </c>
       <c r="D260">
         <v>259</v>
       </c>
@@ -7106,7 +8577,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="261" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A261" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B261" t="s">
+        <v>571</v>
+      </c>
+      <c r="C261">
+        <v>6</v>
+      </c>
       <c r="D261">
         <v>260</v>
       </c>
@@ -7120,7 +8600,16 @@
         <v>753</v>
       </c>
     </row>
-    <row r="262" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A262" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B262" t="s">
+        <v>571</v>
+      </c>
+      <c r="C262">
+        <v>1</v>
+      </c>
       <c r="D262">
         <v>261</v>
       </c>
@@ -7134,7 +8623,16 @@
         <v>1999</v>
       </c>
     </row>
-    <row r="263" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A263" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B263" t="s">
+        <v>571</v>
+      </c>
+      <c r="C263">
+        <v>2</v>
+      </c>
       <c r="D263">
         <v>262</v>
       </c>
@@ -7148,7 +8646,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="264" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A264" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B264" t="s">
+        <v>571</v>
+      </c>
+      <c r="C264">
+        <v>3</v>
+      </c>
       <c r="D264">
         <v>263</v>
       </c>
@@ -7162,7 +8669,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="265" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A265" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B265" t="s">
+        <v>571</v>
+      </c>
+      <c r="C265">
+        <v>4</v>
+      </c>
       <c r="D265">
         <v>264</v>
       </c>
@@ -7176,7 +8692,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="266" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A266" s="1">
+        <v>2.8490030000000001E-3</v>
+      </c>
+      <c r="B266" t="s">
+        <v>571</v>
+      </c>
+      <c r="C266">
+        <v>5</v>
+      </c>
       <c r="D266">
         <v>265</v>
       </c>
@@ -7190,7 +8715,16 @@
         <v>317</v>
       </c>
     </row>
-    <row r="267" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A267" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B267" t="s">
+        <v>572</v>
+      </c>
+      <c r="C267">
+        <v>1</v>
+      </c>
       <c r="D267">
         <v>266</v>
       </c>
@@ -7204,7 +8738,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="268" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A268" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B268" t="s">
+        <v>572</v>
+      </c>
+      <c r="C268">
+        <v>2</v>
+      </c>
       <c r="D268">
         <v>267</v>
       </c>
@@ -7218,7 +8761,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="269" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A269" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B269" t="s">
+        <v>572</v>
+      </c>
+      <c r="C269">
+        <v>3</v>
+      </c>
       <c r="D269">
         <v>268</v>
       </c>
@@ -7232,7 +8784,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="270" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A270" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B270" t="s">
+        <v>572</v>
+      </c>
+      <c r="C270">
+        <v>4</v>
+      </c>
       <c r="D270">
         <v>269</v>
       </c>
@@ -7246,7 +8807,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="271" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A271" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B271" t="s">
+        <v>572</v>
+      </c>
+      <c r="C271">
+        <v>5</v>
+      </c>
       <c r="D271">
         <v>270</v>
       </c>
@@ -7260,7 +8830,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="272" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A272" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B272" t="s">
+        <v>572</v>
+      </c>
+      <c r="C272">
+        <v>6</v>
+      </c>
       <c r="D272">
         <v>271</v>
       </c>
@@ -7274,7 +8853,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="273" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A273" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B273" t="s">
+        <v>572</v>
+      </c>
+      <c r="C273">
+        <v>7</v>
+      </c>
       <c r="D273">
         <v>272</v>
       </c>
@@ -7288,7 +8876,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="274" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A274" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B274" t="s">
+        <v>572</v>
+      </c>
+      <c r="C274">
+        <v>8</v>
+      </c>
       <c r="D274">
         <v>273</v>
       </c>
@@ -7302,7 +8899,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="275" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A275" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B275" t="s">
+        <v>572</v>
+      </c>
+      <c r="C275">
+        <v>9</v>
+      </c>
       <c r="D275">
         <v>274</v>
       </c>
@@ -7316,7 +8922,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="276" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A276" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B276" t="s">
+        <v>572</v>
+      </c>
+      <c r="C276">
+        <v>10</v>
+      </c>
       <c r="D276">
         <v>275</v>
       </c>
@@ -7330,7 +8945,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="277" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A277" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B277" t="s">
+        <v>572</v>
+      </c>
+      <c r="C277">
+        <v>11</v>
+      </c>
       <c r="D277">
         <v>276</v>
       </c>
@@ -7344,7 +8968,16 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="278" spans="4:7" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A278" s="1">
+        <v>6.4102559999999996E-3</v>
+      </c>
+      <c r="B278" t="s">
+        <v>572</v>
+      </c>
+      <c r="C278">
+        <v>12</v>
+      </c>
       <c r="D278">
         <v>277</v>
       </c>
@@ -7360,5 +8993,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>